<commit_message>
Added phd app tracking webpage and made some changes to the variable stars page
</commit_message>
<xml_diff>
--- a/dirlit/webpage/17stars1.xlsx
+++ b/dirlit/webpage/17stars1.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="117">
   <si>
     <t xml:space="preserve">Paper ID</t>
   </si>
@@ -73,6 +73,9 @@
     <t xml:space="preserve">Yashodhan</t>
   </si>
   <si>
+    <t xml:space="preserve">Dr. Alex</t>
+  </si>
+  <si>
     <t xml:space="preserve">-1_-4</t>
   </si>
   <si>
@@ -145,6 +148,9 @@
     <t xml:space="preserve">Not sure what is happening, there seems to be some periodicity, need input.</t>
   </si>
   <si>
+    <t xml:space="preserve">good LB star</t>
+  </si>
+  <si>
     <t xml:space="preserve">00_-3</t>
   </si>
   <si>
@@ -166,6 +172,9 @@
     <t xml:space="preserve">The ZTF match is too far, so ignore the data from ZTF. Looks like an L in our data.</t>
   </si>
   <si>
+    <t xml:space="preserve">not var</t>
+  </si>
+  <si>
     <t xml:space="preserve">22 41 47.89 +50 17 10.8</t>
   </si>
   <si>
@@ -181,6 +190,9 @@
     <t xml:space="preserve">awesome</t>
   </si>
   <si>
+    <t xml:space="preserve">good. Known as var after ATLAS (?).</t>
+  </si>
+  <si>
     <t xml:space="preserve">01_-5</t>
   </si>
   <si>
@@ -217,6 +229,9 @@
     <t xml:space="preserve">A little weak case, but periodicity is seen in all data.</t>
   </si>
   <si>
+    <t xml:space="preserve">dubious, but keep it.</t>
+  </si>
+  <si>
     <t xml:space="preserve">02_-3</t>
   </si>
   <si>
@@ -226,6 +241,9 @@
     <t xml:space="preserve">16-17</t>
   </si>
   <si>
+    <t xml:space="preserve">dubious, but keep it. </t>
+  </si>
+  <si>
     <t xml:space="preserve">02_-4</t>
   </si>
   <si>
@@ -253,6 +271,9 @@
     <t xml:space="preserve">Good L</t>
   </si>
   <si>
+    <t xml:space="preserve">keep marked as LB:</t>
+  </si>
+  <si>
     <t xml:space="preserve">00_-5</t>
   </si>
   <si>
@@ -271,10 +292,13 @@
     <t xml:space="preserve">very interesting, in the flare image the star is actually different</t>
   </si>
   <si>
-    <t xml:space="preserve">Ignore the lightcurve and periodogram here, they are of another star(s) entirely (hence the *). Near this star, in our data we see a flare/nova in some images. Prof. Samus' comment: "very interesting, in the flare image the star is actually different"</t>
-  </si>
-  <si>
-    <t xml:space="preserve">23 36 17.66 +56 48 04.7</t>
+    <t xml:space="preserve">There was another star near this star, this star is not variable. Nothing worth a publication was found even after going through all the photographs.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">is a blend of two stars, red and blue. Not var at all.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">22 36 17.66 +56 48 04.7</t>
   </si>
   <si>
     <t xml:space="preserve">16.3-17.6</t>
@@ -289,6 +313,9 @@
     <t xml:space="preserve">Looks like EW, star not found in ZTF.</t>
   </si>
   <si>
+    <t xml:space="preserve">great EB star with P = 0.595753 d.</t>
+  </si>
+  <si>
     <t xml:space="preserve">02_05</t>
   </si>
   <si>
@@ -320,6 +347,9 @@
   </si>
   <si>
     <t xml:space="preserve">15.2-15.7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">good LB. J-K = 11.375 - 10.557 = 0.818..  https://ztf.snad.space/dr17/view/804211100018212</t>
   </si>
   <si>
     <t xml:space="preserve">22 53 01.41 +48 55 32.6</t>
@@ -475,17 +505,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:Q1000"/>
+  <dimension ref="A1:R1000"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="Q12" activeCellId="0" sqref="Q12"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="Q18" activeCellId="0" sqref="Q18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.640625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.66015625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="4" style="0" width="22.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="11.99"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="24.59"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="24.6"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -540,6 +570,9 @@
       <c r="Q1" s="3" t="s">
         <v>16</v>
       </c>
+      <c r="R1" s="0" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="4" t="n">
@@ -549,10 +582,10 @@
         <v>4186</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E2" s="1" t="n">
         <v>0.02</v>
@@ -567,31 +600,34 @@
         <v>0.55</v>
       </c>
       <c r="I2" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="L2" s="4" t="n">
         <v>0.4</v>
       </c>
       <c r="M2" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="N2" s="4" t="n">
         <v>8</v>
       </c>
       <c r="O2" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="P2" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q2" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="R2" s="3" t="s">
         <v>24</v>
-      </c>
-      <c r="Q2" s="3" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -602,10 +638,10 @@
         <v>349</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E3" s="1" t="n">
         <v>0.02</v>
@@ -620,34 +656,37 @@
         <v>0.46</v>
       </c>
       <c r="I3" s="4" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="L3" s="4" t="n">
         <v>0.47</v>
       </c>
       <c r="M3" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="N3" s="4" t="n">
         <v>8</v>
       </c>
       <c r="O3" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="P3" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="Q3" s="3" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>26</v>
+      </c>
+      <c r="R3" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="4" t="n">
         <v>3</v>
       </c>
@@ -655,47 +694,50 @@
         <v>1681</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="E4" s="1" t="n">
         <v>0.04</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="H4" s="4" t="n">
         <v>0.49</v>
       </c>
       <c r="I4" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="L4" s="4" t="n">
         <v>1.06</v>
       </c>
       <c r="M4" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="N4" s="4" t="n">
         <v>8</v>
       </c>
       <c r="O4" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="P4" s="1"/>
       <c r="Q4" s="3" t="s">
-        <v>40</v>
+        <v>41</v>
+      </c>
+      <c r="R4" s="3" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="79.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -706,50 +748,53 @@
         <v>4088</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="E5" s="1" t="n">
         <v>0.269</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="H5" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="I5" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="K5" s="1" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="L5" s="4" t="n">
         <v>0.75</v>
       </c>
       <c r="M5" s="1" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="N5" s="4" t="n">
         <v>8</v>
       </c>
       <c r="O5" s="1" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="P5" s="1"/>
       <c r="Q5" s="3" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>49</v>
+      </c>
+      <c r="R5" s="0" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="4" t="n">
         <v>5</v>
       </c>
@@ -757,10 +802,10 @@
         <v>3944</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="E6" s="1" t="n">
         <v>0.06</v>
@@ -775,34 +820,37 @@
         <v>1</v>
       </c>
       <c r="I6" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="K6" s="1" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="L6" s="4" t="n">
         <v>0.3</v>
       </c>
       <c r="M6" s="1" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="N6" s="4" t="n">
         <v>8</v>
       </c>
       <c r="O6" s="1" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="P6" s="1" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="Q6" s="3" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="79.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>26</v>
+      </c>
+      <c r="R6" s="3" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="4" t="n">
         <v>6</v>
       </c>
@@ -810,50 +858,53 @@
         <v>2639</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="E7" s="1" t="n">
         <v>0.01</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="G7" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="H7" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="I7" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="K7" s="1" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="L7" s="4" t="n">
-        <v>0.389</v>
+        <v>0.39</v>
       </c>
       <c r="M7" s="1" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="N7" s="4" t="n">
         <v>8</v>
       </c>
       <c r="O7" s="1" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="P7" s="1"/>
       <c r="Q7" s="3" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>61</v>
+      </c>
+      <c r="R7" s="0" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="4" t="n">
         <v>7</v>
       </c>
@@ -861,10 +912,10 @@
         <v>1070</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="E8" s="1" t="n">
         <v>0.06</v>
@@ -873,40 +924,43 @@
         <v>2.59</v>
       </c>
       <c r="G8" s="4" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="H8" s="4" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="I8" s="4" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="K8" s="1" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="L8" s="4" t="n">
-        <v>0.378</v>
+        <v>0.38</v>
       </c>
       <c r="M8" s="1" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="N8" s="4" t="n">
         <v>8</v>
       </c>
       <c r="O8" s="1" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="P8" s="1" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="Q8" s="3" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>68</v>
+      </c>
+      <c r="R8" s="3" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="4" t="n">
         <v>8</v>
       </c>
@@ -914,10 +968,10 @@
         <v>494</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>66</v>
+        <v>71</v>
       </c>
       <c r="E9" s="1" t="n">
         <v>0.08</v>
@@ -932,19 +986,19 @@
         <v>1.33</v>
       </c>
       <c r="I9" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="J9" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="K9" s="1" t="s">
-        <v>67</v>
+        <v>72</v>
       </c>
       <c r="L9" s="4" t="n">
         <v>0.3</v>
       </c>
       <c r="M9" s="1" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="N9" s="4" t="n">
         <v>8</v>
@@ -952,10 +1006,13 @@
       <c r="O9" s="1"/>
       <c r="P9" s="1"/>
       <c r="Q9" s="3" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>26</v>
+      </c>
+      <c r="R9" s="3" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="4" t="n">
         <v>9</v>
       </c>
@@ -963,10 +1020,10 @@
         <v>4139</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>68</v>
+        <v>74</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>69</v>
+        <v>75</v>
       </c>
       <c r="E10" s="1" t="n">
         <v>0.06</v>
@@ -975,25 +1032,25 @@
         <v>1.12</v>
       </c>
       <c r="G10" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="H10" s="4" t="n">
         <v>1.12</v>
       </c>
       <c r="I10" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="J10" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="K10" s="1" t="s">
-        <v>70</v>
+        <v>76</v>
       </c>
       <c r="L10" s="4" t="n">
         <v>0.3</v>
       </c>
       <c r="M10" s="1" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="N10" s="4" t="n">
         <v>8</v>
@@ -1001,10 +1058,13 @@
       <c r="O10" s="1"/>
       <c r="P10" s="1"/>
       <c r="Q10" s="3" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>77</v>
+      </c>
+      <c r="R10" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="4" t="n">
         <v>10</v>
       </c>
@@ -1012,50 +1072,53 @@
         <v>20182</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>72</v>
+        <v>78</v>
       </c>
       <c r="E11" s="1" t="n">
         <v>0.02</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="G11" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="H11" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="I11" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="J11" s="1" t="s">
-        <v>73</v>
+        <v>79</v>
       </c>
       <c r="K11" s="1" t="s">
-        <v>74</v>
+        <v>80</v>
       </c>
       <c r="L11" s="4" t="n">
         <v>0.58</v>
       </c>
       <c r="M11" s="1" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="N11" s="4" t="n">
         <v>7</v>
       </c>
       <c r="O11" s="1" t="s">
-        <v>75</v>
+        <v>81</v>
       </c>
       <c r="P11" s="1"/>
       <c r="Q11" s="3" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="214.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>82</v>
+      </c>
+      <c r="R11" s="3" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="102.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="4" t="n">
         <v>11</v>
       </c>
@@ -1063,47 +1126,50 @@
         <v>20213</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>77</v>
+        <v>84</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>78</v>
+        <v>85</v>
       </c>
       <c r="E12" s="1" t="n">
         <v>0.528</v>
       </c>
       <c r="F12" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="G12" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="H12" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="I12" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="J12" s="1" t="s">
-        <v>79</v>
+        <v>86</v>
       </c>
       <c r="K12" s="1" t="s">
-        <v>80</v>
+        <v>87</v>
       </c>
       <c r="L12" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="M12" s="1" t="s">
-        <v>81</v>
+        <v>88</v>
       </c>
       <c r="N12" s="4" t="n">
         <v>7</v>
       </c>
       <c r="O12" s="1" t="s">
-        <v>82</v>
+        <v>89</v>
       </c>
       <c r="P12" s="1"/>
       <c r="Q12" s="3" t="s">
-        <v>83</v>
+        <v>90</v>
+      </c>
+      <c r="R12" s="3" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1114,52 +1180,55 @@
         <v>2881</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>84</v>
+        <v>92</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="F13" s="4" t="n">
         <v>0.59</v>
       </c>
       <c r="G13" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="H13" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="I13" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="J13" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="K13" s="1" t="s">
-        <v>85</v>
+        <v>93</v>
       </c>
       <c r="L13" s="4" t="n">
         <v>0.39</v>
       </c>
       <c r="M13" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="N13" s="4" t="n">
         <v>7</v>
       </c>
       <c r="O13" s="1" t="s">
-        <v>86</v>
+        <v>94</v>
       </c>
       <c r="P13" s="1" t="s">
-        <v>87</v>
+        <v>95</v>
       </c>
       <c r="Q13" s="3" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>96</v>
+      </c>
+      <c r="R13" s="3" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="4" t="n">
         <v>13</v>
       </c>
@@ -1167,10 +1236,10 @@
         <v>219</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>89</v>
+        <v>98</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>90</v>
+        <v>99</v>
       </c>
       <c r="E14" s="1" t="n">
         <v>0.09</v>
@@ -1179,25 +1248,25 @@
         <v>0.125</v>
       </c>
       <c r="G14" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="H14" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="I14" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="J14" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="K14" s="1" t="s">
-        <v>91</v>
+        <v>100</v>
       </c>
       <c r="L14" s="4" t="n">
         <v>0.367</v>
       </c>
       <c r="M14" s="1" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="N14" s="4" t="n">
         <v>7</v>
@@ -1205,10 +1274,13 @@
       <c r="O14" s="1"/>
       <c r="P14" s="1"/>
       <c r="Q14" s="3" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>101</v>
+      </c>
+      <c r="R14" s="0" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="4" t="n">
         <v>14</v>
       </c>
@@ -1216,37 +1288,37 @@
         <v>2081</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>89</v>
+        <v>98</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>93</v>
+        <v>102</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="F15" s="4" t="n">
         <v>0.99</v>
       </c>
       <c r="G15" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="H15" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="I15" s="5" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="J15" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="K15" s="1" t="s">
-        <v>94</v>
+        <v>103</v>
       </c>
       <c r="L15" s="4" t="n">
         <v>0.7</v>
       </c>
       <c r="M15" s="1" t="s">
-        <v>95</v>
+        <v>104</v>
       </c>
       <c r="N15" s="4" t="n">
         <v>7</v>
@@ -1254,10 +1326,13 @@
       <c r="O15" s="1"/>
       <c r="P15" s="1"/>
       <c r="Q15" s="3" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>105</v>
+      </c>
+      <c r="R15" s="0" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="4" t="n">
         <v>15</v>
       </c>
@@ -1265,35 +1340,35 @@
         <v>1714</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>68</v>
+        <v>74</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>97</v>
+        <v>106</v>
       </c>
       <c r="E16" s="1" t="n">
         <v>0.02</v>
       </c>
       <c r="F16" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="G16" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="H16" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="I16" s="4" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="J16" s="1" t="s">
-        <v>98</v>
+        <v>107</v>
       </c>
       <c r="K16" s="1" t="s">
-        <v>99</v>
+        <v>108</v>
       </c>
       <c r="L16" s="1"/>
       <c r="M16" s="1" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="N16" s="4" t="n">
         <v>7</v>
@@ -1301,10 +1376,13 @@
       <c r="O16" s="1"/>
       <c r="P16" s="1"/>
       <c r="Q16" s="3" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="17" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>82</v>
+      </c>
+      <c r="R16" s="3" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="4" t="n">
         <v>16</v>
       </c>
@@ -1312,10 +1390,10 @@
         <v>104</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>89</v>
+        <v>98</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>100</v>
+        <v>110</v>
       </c>
       <c r="E17" s="1" t="n">
         <v>0.08</v>
@@ -1324,25 +1402,25 @@
         <v>1.99</v>
       </c>
       <c r="G17" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="H17" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="I17" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="J17" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="K17" s="1" t="s">
-        <v>101</v>
+        <v>111</v>
       </c>
       <c r="L17" s="4" t="n">
         <v>0.65</v>
       </c>
       <c r="M17" s="1" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="N17" s="4" t="n">
         <v>6</v>
@@ -1350,10 +1428,13 @@
       <c r="O17" s="1"/>
       <c r="P17" s="1"/>
       <c r="Q17" s="3" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="18" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>101</v>
+      </c>
+      <c r="R17" s="0" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="4" t="n">
         <v>17</v>
       </c>
@@ -1361,10 +1442,10 @@
         <v>136</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>102</v>
+        <v>112</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>103</v>
+        <v>113</v>
       </c>
       <c r="E18" s="1" t="n">
         <v>0.01</v>
@@ -1373,35 +1454,38 @@
         <v>4000</v>
       </c>
       <c r="G18" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="H18" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="I18" s="4" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="J18" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="K18" s="1" t="s">
-        <v>104</v>
+        <v>114</v>
       </c>
       <c r="L18" s="4" t="n">
         <v>0.14</v>
       </c>
       <c r="M18" s="1" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="N18" s="4" t="n">
         <v>5</v>
       </c>
       <c r="O18" s="1" t="s">
-        <v>105</v>
+        <v>115</v>
       </c>
       <c r="P18" s="1"/>
       <c r="Q18" s="3" t="s">
-        <v>106</v>
+        <v>116</v>
+      </c>
+      <c r="R18" s="0" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4351,6 +4435,9 @@
       <c r="Q1000" s="6"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="R16" r:id="rId1" display="https://ztf.snad.space/dr17/view/804211100018212"/>
+  </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>

<commit_message>
Updated the variable stars folder
</commit_message>
<xml_diff>
--- a/dirlit/webpage/17stars1.xlsx
+++ b/dirlit/webpage/17stars1.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="286" uniqueCount="172">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="315" uniqueCount="195">
   <si>
     <t xml:space="preserve">Paper ID</t>
   </si>
@@ -479,7 +479,13 @@
     <t xml:space="preserve">B</t>
   </si>
   <si>
-    <t xml:space="preserve">mpa_data_star_1.dat,</t>
+    <t xml:space="preserve">star_1_lc.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Finding_chart_star_1.jpeg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mpa_data_star_1.dat ZTF_zg_data_star_1.txt ZTF_zr_data_star_1.txt</t>
   </si>
   <si>
     <t xml:space="preserve">DR3 1989573201075344384</t>
@@ -488,36 +494,78 @@
     <t xml:space="preserve">22 42 37.33, +50 37 37.7</t>
   </si>
   <si>
+    <t xml:space="preserve">Star_2_lc.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Finding_chart_star_2.jpeg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mpa_data_star_1.dat ZTF_zg_data_star_1.txt ZTF_zr_data_star_1.txt ZTF_zi_data_star_1.txt </t>
+  </si>
+  <si>
     <t xml:space="preserve">DR3 1989476753287806720</t>
   </si>
   <si>
     <t xml:space="preserve">22 42 16.89, +50 04 04.6</t>
   </si>
   <si>
+    <t xml:space="preserve">Star_3_lc.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Finding_chart_star_3.jpeg</t>
+  </si>
+  <si>
     <t xml:space="preserve">DR3 1989494998308806784</t>
   </si>
   <si>
     <t xml:space="preserve">22 41 47.89, +50 17 10.8</t>
   </si>
   <si>
+    <t xml:space="preserve">Star_5_lc.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Finding_chart_star_5.jpeg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mpa_data_star_1.dat ZTF_zg_data_star_1.txt ZTF_zr_data_star_1.txt </t>
+  </si>
+  <si>
     <t xml:space="preserve">DR3 2007164768650338816</t>
   </si>
   <si>
     <t xml:space="preserve">22 51 05.66, +57 33 21.1</t>
   </si>
   <si>
+    <t xml:space="preserve">Star_6_lc.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Finding_chart_star_6.jpeg</t>
+  </si>
+  <si>
     <t xml:space="preserve">DR3 2007136799822425600</t>
   </si>
   <si>
     <t xml:space="preserve">22 48 55.09, +57 15 19.8</t>
   </si>
   <si>
+    <t xml:space="preserve">Star_7_lc.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Finding_chart_star_7.jpeg</t>
+  </si>
+  <si>
     <t xml:space="preserve">DR3 2002954188866388096</t>
   </si>
   <si>
     <t xml:space="preserve">22 56 35.78, +55 26 53.9</t>
   </si>
   <si>
+    <t xml:space="preserve">Star_8_lc.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Finding_chart_star_8.jpeg</t>
+  </si>
+  <si>
     <t xml:space="preserve">DR3 2007290422213768192</t>
   </si>
   <si>
@@ -527,16 +575,37 @@
     <t xml:space="preserve">LB</t>
   </si>
   <si>
+    <t xml:space="preserve">Star_10_lc.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Finding_chart_star_10.jpeg</t>
+  </si>
+  <si>
     <t xml:space="preserve">DR3 2006886386051006464</t>
   </si>
   <si>
     <t xml:space="preserve">22 36 17.66, +56 48 04.7</t>
   </si>
   <si>
+    <t xml:space="preserve">Star_12_lc.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Finding_chart_star_12.jpeg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mpa_data_star_1.dat </t>
+  </si>
+  <si>
     <t xml:space="preserve">DR3 2009804111948440064</t>
   </si>
   <si>
     <t xml:space="preserve">22 57 45.30, +56 24 24.6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Star_15_lc.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Finding_chart_star_15.jpeg</t>
   </si>
 </sst>
 </file>
@@ -552,6 +621,7 @@
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="0"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -573,6 +643,7 @@
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="0"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="3">
@@ -683,11 +754,11 @@
   </sheetPr>
   <dimension ref="A1:S1000"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G1" colorId="64" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="Q9" activeCellId="0" sqref="Q9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.71484375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="22.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="25.56"/>
@@ -4687,18 +4758,19 @@
   </sheetPr>
   <dimension ref="A1:N11"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G1" colorId="64" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L2" activeCellId="0" sqref="L2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A11" activeCellId="0" sqref="A11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="26.53"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="21.67"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="9" style="0" width="14.31"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="16.81"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="15.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="17.22"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="8.54"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="13.19"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="23.54"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="23.61"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4776,13 +4848,19 @@
       <c r="L2" s="0" t="s">
         <v>152</v>
       </c>
+      <c r="M2" s="0" t="s">
+        <v>153</v>
+      </c>
+      <c r="N2" s="0" t="s">
+        <v>154</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="5" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="D3" s="0" t="s">
         <v>25</v>
@@ -4805,13 +4883,22 @@
       <c r="J3" s="0" t="s">
         <v>140</v>
       </c>
+      <c r="L3" s="0" t="s">
+        <v>157</v>
+      </c>
+      <c r="M3" s="0" t="s">
+        <v>158</v>
+      </c>
+      <c r="N3" s="0" t="s">
+        <v>159</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="5" t="s">
-        <v>155</v>
+        <v>160</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>156</v>
+        <v>161</v>
       </c>
       <c r="D4" s="0" t="s">
         <v>53</v>
@@ -4825,22 +4912,28 @@
       <c r="G4" s="0" t="s">
         <v>151</v>
       </c>
-      <c r="H4" s="0" t="n">
-        <v>0.99</v>
-      </c>
       <c r="I4" s="0" t="n">
         <v>2445644.368</v>
       </c>
       <c r="J4" s="0" t="s">
         <v>140</v>
       </c>
+      <c r="L4" s="0" t="s">
+        <v>162</v>
+      </c>
+      <c r="M4" s="0" t="s">
+        <v>163</v>
+      </c>
+      <c r="N4" s="0" t="s">
+        <v>154</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B5" s="5" t="s">
-        <v>157</v>
+        <v>164</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>158</v>
+        <v>165</v>
       </c>
       <c r="D5" s="0" t="s">
         <v>59</v>
@@ -4863,13 +4956,22 @@
       <c r="J5" s="0" t="s">
         <v>140</v>
       </c>
+      <c r="L5" s="0" t="s">
+        <v>166</v>
+      </c>
+      <c r="M5" s="0" t="s">
+        <v>167</v>
+      </c>
+      <c r="N5" s="0" t="s">
+        <v>168</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B6" s="5" t="s">
-        <v>159</v>
+        <v>169</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>160</v>
+        <v>170</v>
       </c>
       <c r="D6" s="0" t="s">
         <v>53</v>
@@ -4889,13 +4991,22 @@
       <c r="J6" s="0" t="s">
         <v>140</v>
       </c>
+      <c r="L6" s="0" t="s">
+        <v>171</v>
+      </c>
+      <c r="M6" s="0" t="s">
+        <v>172</v>
+      </c>
+      <c r="N6" s="0" t="s">
+        <v>159</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B7" s="5" t="s">
-        <v>161</v>
+        <v>173</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>162</v>
+        <v>174</v>
       </c>
       <c r="D7" s="0" t="s">
         <v>59</v>
@@ -4918,13 +5029,22 @@
       <c r="J7" s="0" t="s">
         <v>140</v>
       </c>
+      <c r="L7" s="0" t="s">
+        <v>175</v>
+      </c>
+      <c r="M7" s="0" t="s">
+        <v>176</v>
+      </c>
+      <c r="N7" s="0" t="s">
+        <v>159</v>
+      </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B8" s="5" t="s">
-        <v>163</v>
+        <v>177</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>164</v>
+        <v>178</v>
       </c>
       <c r="D8" s="0" t="s">
         <v>59</v>
@@ -4947,16 +5067,25 @@
       <c r="J8" s="0" t="s">
         <v>140</v>
       </c>
+      <c r="L8" s="0" t="s">
+        <v>179</v>
+      </c>
+      <c r="M8" s="0" t="s">
+        <v>180</v>
+      </c>
+      <c r="N8" s="0" t="s">
+        <v>154</v>
+      </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B9" s="5" t="s">
-        <v>165</v>
+        <v>181</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>166</v>
+        <v>182</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>167</v>
+        <v>183</v>
       </c>
       <c r="E9" s="0" t="n">
         <v>15.3</v>
@@ -4973,13 +5102,22 @@
       <c r="J9" s="0" t="s">
         <v>140</v>
       </c>
+      <c r="L9" s="0" t="s">
+        <v>184</v>
+      </c>
+      <c r="M9" s="0" t="s">
+        <v>185</v>
+      </c>
+      <c r="N9" s="0" t="s">
+        <v>159</v>
+      </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B10" s="5" t="s">
-        <v>168</v>
+        <v>186</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>169</v>
+        <v>187</v>
       </c>
       <c r="D10" s="0" t="s">
         <v>25</v>
@@ -5002,13 +5140,22 @@
       <c r="J10" s="0" t="s">
         <v>140</v>
       </c>
+      <c r="L10" s="0" t="s">
+        <v>188</v>
+      </c>
+      <c r="M10" s="0" t="s">
+        <v>189</v>
+      </c>
+      <c r="N10" s="0" t="s">
+        <v>190</v>
+      </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B11" s="5" t="s">
-        <v>170</v>
+        <v>191</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>171</v>
+        <v>192</v>
       </c>
       <c r="D11" s="0" t="s">
         <v>53</v>
@@ -5027,6 +5174,15 @@
       </c>
       <c r="J11" s="0" t="s">
         <v>140</v>
+      </c>
+      <c r="L11" s="0" t="s">
+        <v>193</v>
+      </c>
+      <c r="M11" s="0" t="s">
+        <v>194</v>
+      </c>
+      <c r="N11" s="0" t="s">
+        <v>159</v>
       </c>
     </row>
   </sheetData>

</xml_diff>